<commit_message>
Dokonceni kapitoly Vyber technologii
</commit_message>
<xml_diff>
--- a/Tabulky/NamedEntities.xlsx
+++ b/Tabulky/NamedEntities.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ondra\Documents\VŠE\DP\Tabulky\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816276ED-078D-4AD0-B17D-FD5DC009A354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9D655EC-66DA-407D-BBE4-64C34D912FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-3576" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -373,12 +374,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="13">
@@ -605,13 +612,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2074,8 +2081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>